<commit_message>
start create mvp2 branch
</commit_message>
<xml_diff>
--- a/ePICreator/HIPÉRICO ARKOPHARMA.xlsx
+++ b/ePICreator/HIPÉRICO ARKOPHARMA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAB85D1-9994-354D-8C32-8CE6E10D1240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FE9234-E72D-4546-83EF-D4CB7D6C7FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdministrableProductDefinition" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="151">
   <si>
     <t>id</t>
   </si>
@@ -1338,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,6 +1382,9 @@
       </c>
       <c r="E2" t="s">
         <v>128</v>
+      </c>
+      <c r="F2" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1855,7 +1858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>